<commit_message>
Last version of EDA
</commit_message>
<xml_diff>
--- a/data/Resultados.xlsx
+++ b/data/Resultados.xlsx
@@ -13,6 +13,7 @@
     <sheet name="Vista_DiaDeSemana" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Vista_FranjaHoraria" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Vista_TipoDeCalle" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Vista_SexoYVehiculo" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -44565,4 +44566,237 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Vehículo_Víctima</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Femenino</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>(%) Femenino</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>(%) Masculina</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Auto</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>15</v>
+      </c>
+      <c r="C2" t="n">
+        <v>79</v>
+      </c>
+      <c r="D2" t="n">
+        <v>94</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>16.0 %</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>84.0 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Bicicleta</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>8</v>
+      </c>
+      <c r="C3" t="n">
+        <v>21</v>
+      </c>
+      <c r="D3" t="n">
+        <v>29</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>27.6 %</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>72.4 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Cargas</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>7</v>
+      </c>
+      <c r="D4" t="n">
+        <v>7</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0.0 %</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>100.0 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>36</v>
+      </c>
+      <c r="C5" t="n">
+        <v>264</v>
+      </c>
+      <c r="D5" t="n">
+        <v>300</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>12.0 %</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>88.0 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Movil</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0.0 %</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>100.0 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Pasajeros</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>60.0 %</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>40.0 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Peaton</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>103</v>
+      </c>
+      <c r="C8" t="n">
+        <v>163</v>
+      </c>
+      <c r="D8" t="n">
+        <v>266</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>38.7 %</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>61.3 %</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>